<commit_message>
add log files and database editing stuff
</commit_message>
<xml_diff>
--- a/user_database.xlsx
+++ b/user_database.xlsx
@@ -1,34 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apkick/Documents/Programming/Spyder/FakeCFBRefBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D78EF72-570C-9C45-903E-E782B47B247D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89412C6F-D4CA-5944-B2C3-D79CED6338DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="1360" windowWidth="24900" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+  <si>
+    <t>Team Name</t>
+  </si>
+  <si>
+    <t>Team Nickname</t>
+  </si>
   <si>
     <t>Conference</t>
   </si>
@@ -36,6 +34,9 @@
     <t>Discord Name</t>
   </si>
   <si>
+    <t>Coach Name</t>
+  </si>
+  <si>
     <t>Offensive Playbook</t>
   </si>
   <si>
@@ -45,43 +46,28 @@
     <t>Overall Record</t>
   </si>
   <si>
-    <t>Coach Name</t>
-  </si>
-  <si>
     <t>Iowa State</t>
   </si>
   <si>
+    <t>Cyclones</t>
+  </si>
+  <si>
     <t>Big 12</t>
   </si>
   <si>
+    <t>Dick Nutter</t>
+  </si>
+  <si>
+    <t>flexbone</t>
+  </si>
+  <si>
+    <t>4-3</t>
+  </si>
+  <si>
     <t>0-0</t>
   </si>
   <si>
-    <t>Dick Nutter</t>
-  </si>
-  <si>
-    <t>Flexbone</t>
-  </si>
-  <si>
-    <t>4-3</t>
-  </si>
-  <si>
-    <t>Team Name</t>
-  </si>
-  <si>
-    <t>Team Nickname</t>
-  </si>
-  <si>
-    <t>Cyclones</t>
-  </si>
-  <si>
-    <t>Iowa</t>
-  </si>
-  <si>
-    <t>Hawkeyes</t>
-  </si>
-  <si>
-    <t>Big 10</t>
+    <t>Minnesota</t>
   </si>
   <si>
     <t>pm_me_cute_sloths_#5223</t>
@@ -133,10 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,7 +405,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -428,7 +413,7 @@
     <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
@@ -437,54 +422,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" t="s">
         <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -492,25 +477,25 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change command to &
</commit_message>
<xml_diff>
--- a/user_database.xlsx
+++ b/user_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apkick/Documents/Programming/Spyder/FakeCFBRefBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89412C6F-D4CA-5944-B2C3-D79CED6338DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F80082-DB2D-BF4E-A6BA-3F0135E54107}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="1360" windowWidth="24900" windowHeight="14640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Team Name</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>0-0</t>
-  </si>
-  <si>
-    <t>Minnesota</t>
   </si>
   <si>
     <t>pm_me_cute_sloths_#5223</t>
@@ -402,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +454,7 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -469,32 +466,6 @@
         <v>13</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix onside kick issue and halftime issues
</commit_message>
<xml_diff>
--- a/user_database.xlsx
+++ b/user_database.xlsx
@@ -404,13 +404,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col bestFit="1" customWidth="1" max="1" min="1" width="10.83203125"/>
     <col bestFit="1" customWidth="1" max="2" min="2" width="14.1640625"/>
@@ -1556,6 +1556,48 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Springfield</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Springs</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>free conference</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Turts#3627</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Hunter Scott</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>air raid</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>4-4</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>0-0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>